<commit_message>
Okta register and login
</commit_message>
<xml_diff>
--- a/Data Files/WorkData/TestWorkData.xlsx
+++ b/Data Files/WorkData/TestWorkData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t/>
   </si>
@@ -51,6 +51,48 @@
   </si>
   <si>
     <t>APCRGSUb1hB2zeq7EzPk</t>
+  </si>
+  <si>
+    <t>Client ID</t>
+  </si>
+  <si>
+    <t>0oamk2hpnzg3zSZep0h7</t>
+  </si>
+  <si>
+    <t>Client secret</t>
+  </si>
+  <si>
+    <t>ly71nkunldRL-wQCq6ZCdQqzzGijEOlCGF0F2mrj</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>drab-porpoise@example.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Misty-Plover-Real-Cicada-4</t>
+  </si>
+  <si>
+    <t>BOhW6s03Hn7EOHTlYaaE</t>
+  </si>
+  <si>
+    <t>KKAITM7eldKlwLGn01qJ</t>
+  </si>
+  <si>
+    <t>0oamk0pm9fQx125R10h7</t>
+  </si>
+  <si>
+    <t>Vm2-JINkX0t3GYjrQyrbDtNNRhYbur5zA06dcZ8f</t>
+  </si>
+  <si>
+    <t>obnoxious-serval@example.com</t>
+  </si>
+  <si>
+    <t>Outrageous-Teira-Xerothermic-Iguana-2</t>
   </si>
 </sst>
 </file>
@@ -410,13 +452,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>